<commit_message>
End of lessons, restarting MEPD v5
</commit_message>
<xml_diff>
--- a/Leçons/Leçons.xlsx
+++ b/Leçons/Leçons.xlsx
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>